<commit_message>
Added support for sequential strategy + Added more charts to talk with Facu
</commit_message>
<xml_diff>
--- a/Simulator_results/Idle times bar charts.xlsx
+++ b/Simulator_results/Idle times bar charts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27318"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\genar\Proyectos\Paper-Binary-Black-Hole-Algorithm\Simulator_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE38C6A7-4A02-40A8-9823-24C4A457E21C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A30D7AA-6E46-4FDC-A8A4-1D9C63DAE61A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{009BC4F7-527D-4E43-AEA7-B7EFAFCE3FA1}"/>
   </bookViews>
@@ -39,15 +39,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Smart</t>
+    <t>Iteration</t>
   </si>
   <si>
-    <t>Binpacking</t>
+    <t>ED</t>
   </si>
   <si>
-    <t>N-Stars</t>
+    <t>DBP</t>
+  </si>
+  <si>
+    <t>PELADO</t>
   </si>
 </sst>
 </file>
@@ -165,9 +168,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -186,7 +187,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="F77F00"/>
+                <a:srgbClr val="FFC000"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -205,7 +206,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FCBF49"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -224,7 +225,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$A$33:$C$33</c:f>
+                <c:f>Sheet1!$B$33:$D$33</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -242,7 +243,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$A$33:$C$33</c:f>
+                <c:f>Sheet1!$B$33:$D$33</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -274,24 +275,24 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$1:$C$1</c:f>
+              <c:f>Sheet1!$B$1:$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>N-Stars</c:v>
+                  <c:v>ED</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Binpacking</c:v>
+                  <c:v>DBP</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Smart</c:v>
+                  <c:v>PELADO</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$32:$C$32</c:f>
+              <c:f>Sheet1!$B$32:$D$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -482,7 +483,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB" b="1"/>
-                  <a:t>Sum. of execution times</a:t>
+                  <a:t>Idle time</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" b="1" baseline="0"/>
@@ -601,7 +602,1017 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Idle</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> time (seconds)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ED</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>99719.714000000007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75212.324999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>84718.084000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>73789.804000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>65773.551999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>98331.146999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>104546.30100000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>62900.892</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80286.392000000007</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>101162.899</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>64809.362999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>93773.678</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>82304.828999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>56055.525000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>79529.409</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>76326.081000000006</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>73554.304000000004</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90043.027000000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>84667.865999999995</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>56681.927000000003</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>102367.514</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>67854.271999999997</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>68771.297000000006</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>84842.438999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>81750.486999999994</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>80393.539000000004</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>101513.49</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>85595.441999999995</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>124135.988</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>92690.206999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-57A5-439A-A688-E1F4BFCD8CF7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DBP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>56851.696000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55191.519999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55341.101000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58024.055999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>58715.559000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>57845.277999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>59067.618999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>60487.925999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>58417.536999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>59799.858</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>61308.879000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>58918.332000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>58013.360999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>57214.485000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>59552.868999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>60513.815000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>59543.993999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>58537.673999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>55754.824000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>56241.874000000003</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>59439.366000000002</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>61116.349000000002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>57213.15</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>58948.896000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>57803.766000000003</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>57617.824999999997</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>61697.527999999998</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>60329.635000000002</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>59007.544999999998</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>58467.942999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-57A5-439A-A688-E1F4BFCD8CF7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PELADO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>90498.053</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23122.345000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23353.710999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23687.262999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22740.253000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22469.891</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22078.466</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23045.289000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21953.733</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50115.502</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22248.692999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22401.269</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>23637.608</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>22234.058000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>22931.781999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>23433.64</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>23329.319</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>23933.292000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>23027.03</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>22908.847000000002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>23614.025000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>23333.776999999998</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23656.045999999998</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>27348.519</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>22513.534</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>23222.975999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>22280.484</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>23133.623</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>21433.24</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>28501.036</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-57A5-439A-A688-E1F4BFCD8CF7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="999389840"/>
+        <c:axId val="999382896"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="999389840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="999382896"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="999382896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="999389840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1144,17 +2155,533 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>451757</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>163286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>451757</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>130629</xdr:rowOff>
@@ -1184,6 +2711,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>106135</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>160564</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>106135</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>127907</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31AEC865-477B-51EE-AAB6-4A28F18B2F04}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1199,35 +2762,455 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="1">
-          <cell r="A1" t="str">
-            <v>N-Stars</v>
-          </cell>
           <cell r="B1" t="str">
-            <v>Binpacking</v>
+            <v>ED</v>
           </cell>
           <cell r="C1" t="str">
-            <v>Smart</v>
+            <v>DBP</v>
+          </cell>
+          <cell r="D1" t="str">
+            <v>PELADO</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2">
+            <v>1</v>
+          </cell>
+          <cell r="B2">
+            <v>208860.982088399</v>
+          </cell>
+          <cell r="C2">
+            <v>166742.79882348599</v>
+          </cell>
+          <cell r="D2">
+            <v>200821.92072227699</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>2</v>
+          </cell>
+          <cell r="B3">
+            <v>180973.03096008301</v>
+          </cell>
+          <cell r="C3">
+            <v>161558.94209641</v>
+          </cell>
+          <cell r="D3">
+            <v>126689.325102028</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>3</v>
+          </cell>
+          <cell r="B4">
+            <v>191676.677469952</v>
+          </cell>
+          <cell r="C4">
+            <v>162259.88219206501</v>
+          </cell>
+          <cell r="D4">
+            <v>127483.26462069299</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>4</v>
+          </cell>
+          <cell r="B5">
+            <v>184906.62866054999</v>
+          </cell>
+          <cell r="C5">
+            <v>169791.11324439</v>
+          </cell>
+          <cell r="D5">
+            <v>132649.89923239601</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>5</v>
+          </cell>
+          <cell r="B6">
+            <v>177349.099754011</v>
+          </cell>
+          <cell r="C6">
+            <v>170876.106512848</v>
+          </cell>
+          <cell r="D6">
+            <v>132000.62548285801</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>6</v>
+          </cell>
+          <cell r="B7">
+            <v>209564.85080439801</v>
+          </cell>
+          <cell r="C7">
+            <v>168253.17834164001</v>
+          </cell>
+          <cell r="D7">
+            <v>130102.748368826</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>7</v>
+          </cell>
+          <cell r="B8">
+            <v>217880.425998583</v>
+          </cell>
+          <cell r="C8">
+            <v>172882.48295372599</v>
+          </cell>
+          <cell r="D8">
+            <v>133018.45250136399</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>8</v>
+          </cell>
+          <cell r="B9">
+            <v>177565.17612346599</v>
+          </cell>
+          <cell r="C9">
+            <v>176788.45872017299</v>
+          </cell>
+          <cell r="D9">
+            <v>136354.37624898701</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>9</v>
+          </cell>
+          <cell r="B10">
+            <v>192854.703273383</v>
+          </cell>
+          <cell r="C10">
+            <v>170900.21747436901</v>
+          </cell>
+          <cell r="D10">
+            <v>131602.794617757</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>10</v>
+          </cell>
+          <cell r="B11">
+            <v>215391.83032727899</v>
+          </cell>
+          <cell r="C11">
+            <v>175338.35660582199</v>
+          </cell>
+          <cell r="D11">
+            <v>163100.630178133</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>11</v>
+          </cell>
+          <cell r="B12">
+            <v>181598.59554366799</v>
+          </cell>
+          <cell r="C12">
+            <v>178689.78025728001</v>
+          </cell>
+          <cell r="D12">
+            <v>136933.039325497</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13">
+            <v>12</v>
+          </cell>
+          <cell r="B13">
+            <v>210969.19109966201</v>
+          </cell>
+          <cell r="C13">
+            <v>175362.467567343</v>
+          </cell>
+          <cell r="D13">
+            <v>135896.26798008199</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14">
+            <v>13</v>
+          </cell>
+          <cell r="B14">
+            <v>193719.520342723</v>
+          </cell>
+          <cell r="C14">
+            <v>169172.839302523</v>
+          </cell>
+          <cell r="D14">
+            <v>131854.23750219401</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15">
+            <v>14</v>
+          </cell>
+          <cell r="B15">
+            <v>165358.191813254</v>
+          </cell>
+          <cell r="C15">
+            <v>167838.12536116701</v>
+          </cell>
+          <cell r="D15">
+            <v>129899.52740743299</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16">
+            <v>15</v>
+          </cell>
+          <cell r="B16">
+            <v>195830.71060146601</v>
+          </cell>
+          <cell r="C16">
+            <v>175226.41285590199</v>
+          </cell>
+          <cell r="D16">
+            <v>135947.934326199</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17">
+            <v>16</v>
+          </cell>
+          <cell r="B17">
+            <v>192485.126550738</v>
+          </cell>
+          <cell r="C17">
+            <v>176953.791027748</v>
+          </cell>
+          <cell r="D17">
+            <v>136908.92836397601</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18">
+            <v>17</v>
+          </cell>
+          <cell r="B18">
+            <v>188083.62933190601</v>
+          </cell>
+          <cell r="C18">
+            <v>174416.97343340199</v>
+          </cell>
+          <cell r="D18">
+            <v>135262.49413437999</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19">
+            <v>18</v>
+          </cell>
+          <cell r="B19">
+            <v>204062.693964306</v>
+          </cell>
+          <cell r="C19">
+            <v>171241.215358741</v>
+          </cell>
+          <cell r="D19">
+            <v>133628.11538554501</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20">
+            <v>19</v>
+          </cell>
+          <cell r="B20">
+            <v>193412.96668909601</v>
+          </cell>
+          <cell r="C20">
+            <v>164366.14690210199</v>
+          </cell>
+          <cell r="D20">
+            <v>129286.420100177</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21">
+            <v>20</v>
+          </cell>
+          <cell r="B21">
+            <v>165838.13764788699</v>
+          </cell>
+          <cell r="C21">
+            <v>165792.138054932</v>
+          </cell>
+          <cell r="D21">
+            <v>129543.029619225</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22">
+            <v>21</v>
+          </cell>
+          <cell r="B22">
+            <v>217991.87148665401</v>
+          </cell>
+          <cell r="C22">
+            <v>173771.144106939</v>
+          </cell>
+          <cell r="D22">
+            <v>135069.60644221</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23">
+            <v>22</v>
+          </cell>
+          <cell r="B23">
+            <v>185091.24054118001</v>
+          </cell>
+          <cell r="C23">
+            <v>178965.33410323699</v>
+          </cell>
+          <cell r="D23">
+            <v>138045.58797855099</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24">
+            <v>23</v>
+          </cell>
+          <cell r="B24">
+            <v>180105.956238218</v>
+          </cell>
+          <cell r="C24">
+            <v>168420.232860752</v>
+          </cell>
+          <cell r="D24">
+            <v>131924.84817521999</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25">
+            <v>24</v>
+          </cell>
+          <cell r="B25">
+            <v>200191.58594872299</v>
+          </cell>
+          <cell r="C25">
+            <v>174189.64151048701</v>
+          </cell>
+          <cell r="D25">
+            <v>139489</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26">
+            <v>25</v>
+          </cell>
+          <cell r="B26">
+            <v>193484.96357717901</v>
+          </cell>
+          <cell r="C26">
+            <v>169128.06180255499</v>
+          </cell>
+          <cell r="D26">
+            <v>130857.077022135</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27">
+            <v>26</v>
+          </cell>
+          <cell r="B27">
+            <v>190260.012640206</v>
+          </cell>
+          <cell r="C27">
+            <v>167538.460553688</v>
+          </cell>
+          <cell r="D27">
+            <v>130726.188945305</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28">
+            <v>27</v>
+          </cell>
+          <cell r="B28">
+            <v>219492.27553722999</v>
+          </cell>
+          <cell r="C28">
+            <v>180472.26919831699</v>
+          </cell>
+          <cell r="D28">
+            <v>137978.421728599</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29">
+            <v>28</v>
+          </cell>
+          <cell r="B29">
+            <v>201720.89255060599</v>
+          </cell>
+          <cell r="C29">
+            <v>176168.46256676901</v>
+          </cell>
+          <cell r="D29">
+            <v>136016.82278768899</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30">
+            <v>29</v>
+          </cell>
+          <cell r="B30">
+            <v>238127.47145375799</v>
+          </cell>
+          <cell r="C30">
+            <v>172488.096511699</v>
+          </cell>
+          <cell r="D30">
+            <v>132010.95875208199</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31">
+            <v>30</v>
+          </cell>
+          <cell r="B31">
+            <v>206124.61004542201</v>
+          </cell>
+          <cell r="C31">
+            <v>171671.76824305</v>
+          </cell>
+          <cell r="D31">
+            <v>138682</v>
           </cell>
         </row>
         <row r="32">
-          <cell r="A32">
+          <cell r="B32">
             <v>196032.4349687995</v>
           </cell>
-          <cell r="B32">
+          <cell r="C32">
             <v>171575.49661811872</v>
           </cell>
-          <cell r="C32">
+          <cell r="D32">
             <v>136659.48476839394</v>
           </cell>
         </row>
         <row r="33">
-          <cell r="A33">
+          <cell r="B33">
             <v>16687.153226153521</v>
           </cell>
-          <cell r="B33">
+          <cell r="C33">
             <v>4873.6862446526629</v>
           </cell>
-          <cell r="C33">
+          <cell r="D33">
             <v>13692.444736183112</v>
           </cell>
         </row>
@@ -1554,384 +3537,477 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DB5940F-EA65-4BAB-A6F9-F49C179449AD}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" topLeftCell="F5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="19.3046875" customWidth="1"/>
-    <col min="2" max="2" width="25.3828125" customWidth="1"/>
-    <col min="3" max="3" width="20.3046875" customWidth="1"/>
+    <col min="2" max="2" width="19.3046875" customWidth="1"/>
+    <col min="3" max="3" width="25.3828125" customWidth="1"/>
+    <col min="4" max="4" width="20.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>99719.714000000007</v>
       </c>
-      <c r="B2" s="3">
+      <c r="C2" s="3">
         <v>56851.696000000004</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>90498.053</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
         <v>75212.324999999997</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>55191.519999999997</v>
       </c>
-      <c r="C3" s="3">
+      <c r="D3" s="3">
         <v>23122.345000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
         <v>84718.084000000003</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>55341.101000000002</v>
       </c>
-      <c r="C4" s="3">
+      <c r="D4" s="3">
         <v>23353.710999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
         <v>73789.804000000004</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>58024.055999999997</v>
       </c>
-      <c r="C5" s="3">
+      <c r="D5" s="3">
         <v>23687.262999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
         <v>65773.551999999996</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>58715.559000000001</v>
       </c>
-      <c r="C6" s="3">
+      <c r="D6" s="3">
         <v>22740.253000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
         <v>98331.146999999997</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>57845.277999999998</v>
       </c>
-      <c r="C7" s="3">
+      <c r="D7" s="3">
         <v>22469.891</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
         <v>104546.30100000001</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>59067.618999999999</v>
       </c>
-      <c r="C8" s="3">
+      <c r="D8" s="3">
         <v>22078.466</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
         <v>62900.892</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>60487.925999999999</v>
       </c>
-      <c r="C9" s="3">
+      <c r="D9" s="3">
         <v>23045.289000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
         <v>80286.392000000007</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>58417.536999999997</v>
       </c>
-      <c r="C10" s="3">
+      <c r="D10" s="3">
         <v>21953.733</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
         <v>101162.899</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>59799.858</v>
       </c>
-      <c r="C11" s="3">
+      <c r="D11" s="3">
         <v>50115.502</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
         <v>64809.362999999998</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>61308.879000000001</v>
       </c>
-      <c r="C12" s="3">
+      <c r="D12" s="3">
         <v>22248.692999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
         <v>93773.678</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>58918.332000000002</v>
       </c>
-      <c r="C13" s="3">
+      <c r="D13" s="3">
         <v>22401.269</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
         <v>82304.828999999998</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>58013.360999999997</v>
       </c>
-      <c r="C14" s="3">
+      <c r="D14" s="3">
         <v>23637.608</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
         <v>56055.525000000001</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>57214.485000000001</v>
       </c>
-      <c r="C15" s="3">
+      <c r="D15" s="3">
         <v>22234.058000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
         <v>79529.409</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>59552.868999999999</v>
       </c>
-      <c r="C16" s="3">
+      <c r="D16" s="3">
         <v>22931.781999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
         <v>76326.081000000006</v>
       </c>
-      <c r="B17">
+      <c r="C17">
         <v>60513.815000000002</v>
       </c>
-      <c r="C17" s="3">
+      <c r="D17" s="3">
         <v>23433.64</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
         <v>73554.304000000004</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <v>59543.993999999999</v>
       </c>
-      <c r="C18" s="3">
+      <c r="D18" s="3">
         <v>23329.319</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
         <v>90043.027000000002</v>
       </c>
-      <c r="B19">
+      <c r="C19">
         <v>58537.673999999999</v>
       </c>
-      <c r="C19" s="3">
+      <c r="D19" s="3">
         <v>23933.292000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
         <v>84667.865999999995</v>
       </c>
-      <c r="B20">
+      <c r="C20">
         <v>55754.824000000001</v>
       </c>
-      <c r="C20" s="3">
+      <c r="D20" s="3">
         <v>23027.03</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
         <v>56681.927000000003</v>
       </c>
-      <c r="B21">
+      <c r="C21">
         <v>56241.874000000003</v>
       </c>
-      <c r="C21" s="3">
+      <c r="D21" s="3">
         <v>22908.847000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
         <v>102367.514</v>
       </c>
-      <c r="B22">
+      <c r="C22">
         <v>59439.366000000002</v>
       </c>
-      <c r="C22" s="3">
+      <c r="D22" s="3">
         <v>23614.025000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
         <v>67854.271999999997</v>
       </c>
-      <c r="B23">
+      <c r="C23">
         <v>61116.349000000002</v>
       </c>
-      <c r="C23" s="3">
+      <c r="D23" s="3">
         <v>23333.776999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
         <v>68771.297000000006</v>
       </c>
-      <c r="B24">
+      <c r="C24">
         <v>57213.15</v>
       </c>
-      <c r="C24" s="3">
+      <c r="D24" s="3">
         <v>23656.045999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
         <v>84842.438999999998</v>
       </c>
-      <c r="B25">
+      <c r="C25">
         <v>58948.896000000001</v>
       </c>
-      <c r="C25" s="3">
+      <c r="D25" s="3">
         <v>27348.519</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
         <v>81750.486999999994</v>
       </c>
-      <c r="B26">
+      <c r="C26">
         <v>57803.766000000003</v>
       </c>
-      <c r="C26" s="3">
+      <c r="D26" s="3">
         <v>22513.534</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
         <v>80393.539000000004</v>
       </c>
-      <c r="B27">
+      <c r="C27">
         <v>57617.824999999997</v>
       </c>
-      <c r="C27" s="3">
+      <c r="D27" s="3">
         <v>23222.975999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
         <v>101513.49</v>
       </c>
-      <c r="B28">
+      <c r="C28">
         <v>61697.527999999998</v>
       </c>
-      <c r="C28" s="3">
+      <c r="D28" s="3">
         <v>22280.484</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
         <v>85595.441999999995</v>
       </c>
-      <c r="B29">
+      <c r="C29">
         <v>60329.635000000002</v>
       </c>
-      <c r="C29" s="3">
+      <c r="D29" s="3">
         <v>23133.623</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
         <v>124135.988</v>
       </c>
-      <c r="B30">
+      <c r="C30">
         <v>59007.544999999998</v>
       </c>
-      <c r="C30" s="3">
+      <c r="D30" s="3">
         <v>21433.24</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
         <v>92690.206999999995</v>
       </c>
-      <c r="B31">
+      <c r="C31">
         <v>58467.942999999999</v>
       </c>
-      <c r="C31" s="3">
+      <c r="D31" s="3">
         <v>28501.036</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A32" s="1">
-        <f>AVERAGE(A2:A31)</f>
-        <v>83136.72646666666</v>
-      </c>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B32" s="1">
         <f>AVERAGE(B2:B31)</f>
-        <v>58566.141999999985</v>
+        <v>83136.72646666666</v>
       </c>
       <c r="C32" s="1">
         <f>AVERAGE(C2:C31)</f>
+        <v>58566.141999999985</v>
+      </c>
+      <c r="D32" s="1">
+        <f>AVERAGE(D2:D31)</f>
         <v>26406.243466666667</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A33" s="2">
-        <f>STDEV(A2:A31)</f>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B33" s="2">
+        <f>STDEV(B2:B31)</f>
         <v>15738.411131354378</v>
       </c>
-      <c r="B33" s="2">
-        <f t="shared" ref="B33:C33" si="0">STDEV(B2:B31)</f>
+      <c r="C33" s="2">
+        <f t="shared" ref="C33:D33" si="0">STDEV(C2:C31)</f>
         <v>1698.9410735642525</v>
       </c>
-      <c r="C33" s="2">
+      <c r="D33" s="2">
         <f t="shared" si="0"/>
         <v>13133.969509412373</v>
       </c>

</xml_diff>